<commit_message>
Add mas censistas excel y visualizacion resultados del algortimo goloso
</commit_message>
<xml_diff>
--- a/src/listas_de_censistas/datosPruebaCensistas.xlsx
+++ b/src/listas_de_censistas/datosPruebaCensistas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -33,7 +33,16 @@
     <t>Paula</t>
   </si>
   <si>
-    <t>Tito</t>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Juana</t>
+  </si>
+  <si>
+    <t>Vanesa</t>
+  </si>
+  <si>
+    <t>Diego</t>
   </si>
 </sst>
 </file>
@@ -111,15 +120,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:colOff>1343025</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85344</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -142,8 +151,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1066800" y="1752600"/>
-          <a:ext cx="800100" cy="657226"/>
+          <a:off x="1152525" y="343281"/>
+          <a:ext cx="800100" cy="504063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -155,15 +164,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:colOff>1295400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -186,8 +195,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1057275" y="971550"/>
-          <a:ext cx="838200" cy="695325"/>
+          <a:off x="1066800" y="1057276"/>
+          <a:ext cx="838200" cy="571500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -199,15 +208,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -230,7 +239,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1133476" y="257175"/>
+          <a:off x="1238251" y="1752600"/>
           <a:ext cx="723899" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -240,6 +249,123 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>124206</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="800100" cy="504063"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076325" y="2600706"/>
+          <a:ext cx="800100" cy="504063"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>518573</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="658303" cy="581025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1128173" y="3352800"/>
+          <a:ext cx="658303" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514888</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="657226" cy="657226"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1124488" y="4067175"/>
+          <a:ext cx="657226" cy="657226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -506,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,14 +705,74 @@
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>